<commit_message>
More work on udp app
</commit_message>
<xml_diff>
--- a/artifacts/f12017/udp.xlsx
+++ b/artifacts/f12017/udp.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="109">
   <si>
     <t xml:space="preserve">    float m_lapDistance;</t>
   </si>
@@ -340,6 +340,9 @@
   </si>
   <si>
     <t xml:space="preserve">CarUDPData  m_car_data[20]; </t>
+  </si>
+  <si>
+    <t>End (exclusive)</t>
   </si>
 </sst>
 </file>
@@ -690,19 +693,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E106"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="28.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -710,8 +714,9 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -719,1595 +724,1930 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3">
+        <f>B3+F3</f>
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <f>IF(D3="float",4,IF(D3="byte",1,"Error"))</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <f>IF(E3="float",4,IF(E3="byte",1,"Error"))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
-        <f>B3+E3</f>
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
+        <f>B3+F3</f>
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C67" si="0">B4+F4</f>
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E67" si="0">IF(D4="float",4,IF(D4="byte",1,"Error"))</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F67" si="1">IF(E4="float",4,IF(E4="byte",1,"Error"))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:B68" si="1">B4+E4</f>
+        <f t="shared" ref="B5:B68" si="2">B4+F4</f>
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="B8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
       <c r="B10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
         <v>16</v>
       </c>
-      <c r="D10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
       <c r="B11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
         <v>17</v>
       </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
       <c r="B12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
         <v>18</v>
       </c>
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
       <c r="B13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
         <v>19</v>
       </c>
-      <c r="D13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
       <c r="B14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
         <v>20</v>
       </c>
-      <c r="D14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
       <c r="B15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
         <v>21</v>
       </c>
-      <c r="D15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
       <c r="B16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="D16" t="s">
         <v>22</v>
       </c>
-      <c r="D16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
       <c r="B17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>56</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="D17" t="s">
         <v>23</v>
       </c>
-      <c r="D17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
       <c r="B18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
         <v>24</v>
       </c>
-      <c r="D18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
       <c r="B19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="D19" t="s">
         <v>25</v>
       </c>
-      <c r="D19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
       <c r="B20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>68</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="D20" t="s">
         <v>26</v>
       </c>
-      <c r="D20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20">
-        <f>IF(D20="float",4,IF(D20="byte",1,"Error"))*4</f>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <f>IF(E20="float",4,IF(E20="byte",1,"Error"))*4</f>
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
       <c r="B21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>84</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="D21" t="s">
         <v>27</v>
       </c>
-      <c r="D21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21">
-        <f>IF(D21="float",4,IF(D21="byte",1,"Error"))*4</f>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <f>IF(E21="float",4,IF(E21="byte",1,"Error"))*4</f>
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
       <c r="B22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+      <c r="D22" t="s">
         <v>28</v>
       </c>
-      <c r="D22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22">
-        <f>IF(D22="float",4,IF(D22="byte",1,"Error"))*4</f>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <f>IF(E22="float",4,IF(E22="byte",1,"Error"))*4</f>
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
       <c r="B23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>116</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="D23" t="s">
         <v>29</v>
       </c>
-      <c r="D23" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
       <c r="B24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="D24" t="s">
         <v>30</v>
       </c>
-      <c r="D24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
       <c r="B25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>124</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+      <c r="D25" t="s">
         <v>31</v>
       </c>
-      <c r="D25" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
       <c r="B26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>128</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>132</v>
+      </c>
+      <c r="D26" t="s">
         <v>32</v>
       </c>
-      <c r="D26" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24</v>
       </c>
       <c r="B27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>132</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>136</v>
+      </c>
+      <c r="D27" t="s">
         <v>33</v>
       </c>
-      <c r="D27" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>25</v>
       </c>
       <c r="B28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>136</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="D28" t="s">
         <v>34</v>
       </c>
-      <c r="D28" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>26</v>
       </c>
       <c r="B29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>140</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="D29" t="s">
         <v>35</v>
       </c>
-      <c r="D29" t="s">
-        <v>4</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
       <c r="B30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>144</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>148</v>
+      </c>
+      <c r="D30" t="s">
         <v>36</v>
       </c>
-      <c r="D30" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
       <c r="B31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>148</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>152</v>
+      </c>
+      <c r="D31" t="s">
         <v>37</v>
       </c>
-      <c r="D31" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>29</v>
       </c>
       <c r="B32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>152</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>156</v>
+      </c>
+      <c r="D32" t="s">
         <v>38</v>
       </c>
-      <c r="D32" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>30</v>
       </c>
       <c r="B33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>156</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="D33" t="s">
         <v>39</v>
       </c>
-      <c r="D33" t="s">
-        <v>4</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>31</v>
       </c>
       <c r="B34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>160</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>164</v>
+      </c>
+      <c r="D34" t="s">
         <v>40</v>
       </c>
-      <c r="D34" t="s">
-        <v>4</v>
-      </c>
-      <c r="E34">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>32</v>
       </c>
       <c r="B35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>164</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>168</v>
+      </c>
+      <c r="D35" t="s">
         <v>41</v>
       </c>
-      <c r="D35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>33</v>
       </c>
       <c r="B36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>168</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>172</v>
+      </c>
+      <c r="D36" t="s">
         <v>42</v>
       </c>
-      <c r="D36" t="s">
-        <v>4</v>
-      </c>
-      <c r="E36">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>34</v>
       </c>
       <c r="B37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>172</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>176</v>
+      </c>
+      <c r="D37" t="s">
         <v>43</v>
       </c>
-      <c r="D37" t="s">
-        <v>4</v>
-      </c>
-      <c r="E37">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>35</v>
       </c>
       <c r="B38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>176</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="D38" t="s">
         <v>44</v>
       </c>
-      <c r="D38" t="s">
-        <v>4</v>
-      </c>
-      <c r="E38">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>36</v>
       </c>
       <c r="B39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>184</v>
+      </c>
+      <c r="D39" t="s">
         <v>45</v>
       </c>
-      <c r="D39" t="s">
-        <v>4</v>
-      </c>
-      <c r="E39">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>37</v>
       </c>
       <c r="B40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>184</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>188</v>
+      </c>
+      <c r="D40" t="s">
         <v>46</v>
       </c>
-      <c r="D40" t="s">
-        <v>4</v>
-      </c>
-      <c r="E40">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>38</v>
       </c>
       <c r="B41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>188</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>192</v>
+      </c>
+      <c r="D41" t="s">
         <v>47</v>
       </c>
-      <c r="D41" t="s">
-        <v>4</v>
-      </c>
-      <c r="E41">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>39</v>
       </c>
       <c r="B42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>192</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>196</v>
+      </c>
+      <c r="D42" t="s">
         <v>48</v>
       </c>
-      <c r="D42" t="s">
-        <v>4</v>
-      </c>
-      <c r="E42">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>40</v>
       </c>
       <c r="B43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>196</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="D43" t="s">
         <v>49</v>
       </c>
-      <c r="D43" t="s">
-        <v>4</v>
-      </c>
-      <c r="E43">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>41</v>
       </c>
       <c r="B44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>204</v>
+      </c>
+      <c r="D44" t="s">
         <v>50</v>
       </c>
-      <c r="D44" t="s">
-        <v>4</v>
-      </c>
-      <c r="E44">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>42</v>
       </c>
       <c r="B45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>204</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>220</v>
+      </c>
+      <c r="D45" t="s">
         <v>51</v>
       </c>
-      <c r="D45" t="s">
-        <v>4</v>
-      </c>
-      <c r="E45">
-        <f>IF(D45="float",4,IF(D45="byte",1,"Error"))*4</f>
+      <c r="E45" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45">
+        <f>IF(E45="float",4,IF(E45="byte",1,"Error"))*4</f>
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>43</v>
       </c>
       <c r="B46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>220</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>236</v>
+      </c>
+      <c r="D46" t="s">
         <v>52</v>
       </c>
-      <c r="D46" t="s">
-        <v>4</v>
-      </c>
-      <c r="E46">
-        <f>IF(D46="float",4,IF(D46="byte",1,"Error"))*4</f>
+      <c r="E46" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46">
+        <f>IF(E46="float",4,IF(E46="byte",1,"Error"))*4</f>
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>44</v>
       </c>
       <c r="B47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>236</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="D47" t="s">
         <v>53</v>
       </c>
-      <c r="D47" t="s">
-        <v>4</v>
-      </c>
-      <c r="E47">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>4</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>45</v>
       </c>
       <c r="B48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>240</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>244</v>
+      </c>
+      <c r="D48" t="s">
         <v>54</v>
       </c>
-      <c r="D48" t="s">
-        <v>4</v>
-      </c>
-      <c r="E48">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>4</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>46</v>
       </c>
       <c r="B49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>248</v>
+      </c>
+      <c r="D49" t="s">
         <v>55</v>
       </c>
-      <c r="D49" t="s">
-        <v>4</v>
-      </c>
-      <c r="E49">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>47</v>
       </c>
       <c r="B50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>248</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>252</v>
+      </c>
+      <c r="D50" t="s">
         <v>56</v>
       </c>
-      <c r="D50" t="s">
-        <v>4</v>
-      </c>
-      <c r="E50">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>48</v>
       </c>
       <c r="B51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>252</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>256</v>
+      </c>
+      <c r="D51" t="s">
         <v>57</v>
       </c>
-      <c r="D51" t="s">
-        <v>4</v>
-      </c>
-      <c r="E51">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>4</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>49</v>
       </c>
       <c r="B52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>256</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>260</v>
+      </c>
+      <c r="D52" t="s">
         <v>58</v>
       </c>
-      <c r="D52" t="s">
-        <v>4</v>
-      </c>
-      <c r="E52">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>4</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>50</v>
       </c>
       <c r="B53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>260</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>264</v>
+      </c>
+      <c r="D53" t="s">
         <v>59</v>
       </c>
-      <c r="D53" t="s">
-        <v>4</v>
-      </c>
-      <c r="E53">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>51</v>
       </c>
       <c r="B54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>264</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>268</v>
+      </c>
+      <c r="D54" t="s">
         <v>60</v>
       </c>
-      <c r="D54" t="s">
-        <v>4</v>
-      </c>
-      <c r="E54">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>52</v>
       </c>
       <c r="B55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>268</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>272</v>
+      </c>
+      <c r="D55" t="s">
         <v>61</v>
       </c>
-      <c r="D55" t="s">
-        <v>4</v>
-      </c>
-      <c r="E55">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>4</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>53</v>
       </c>
       <c r="B56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>272</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>276</v>
+      </c>
+      <c r="D56" t="s">
         <v>62</v>
       </c>
-      <c r="D56" t="s">
-        <v>4</v>
-      </c>
-      <c r="E56">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>4</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>54</v>
       </c>
       <c r="B57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>276</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
+      <c r="D57" t="s">
         <v>63</v>
       </c>
-      <c r="D57" t="s">
-        <v>4</v>
-      </c>
-      <c r="E57">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>4</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>55</v>
       </c>
       <c r="B58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>280</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>284</v>
+      </c>
+      <c r="D58" t="s">
         <v>64</v>
       </c>
-      <c r="D58" t="s">
-        <v>4</v>
-      </c>
-      <c r="E58">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E58" t="s">
+        <v>4</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>56</v>
       </c>
       <c r="B59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>284</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>288</v>
+      </c>
+      <c r="D59" t="s">
         <v>65</v>
       </c>
-      <c r="D59" t="s">
-        <v>4</v>
-      </c>
-      <c r="E59">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
+        <v>4</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>57</v>
       </c>
       <c r="B60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>288</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>292</v>
+      </c>
+      <c r="D60" t="s">
         <v>66</v>
       </c>
-      <c r="D60" t="s">
-        <v>4</v>
-      </c>
-      <c r="E60">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>4</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>58</v>
       </c>
       <c r="B61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>292</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>296</v>
+      </c>
+      <c r="D61" t="s">
         <v>67</v>
       </c>
-      <c r="D61" t="s">
-        <v>4</v>
-      </c>
-      <c r="E61">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>4</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>59</v>
       </c>
       <c r="B62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>296</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="D62" t="s">
         <v>68</v>
       </c>
-      <c r="D62" t="s">
-        <v>4</v>
-      </c>
-      <c r="E62">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>4</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>60</v>
       </c>
       <c r="B63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>300</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>304</v>
+      </c>
+      <c r="D63" t="s">
         <v>69</v>
       </c>
-      <c r="D63" t="s">
-        <v>4</v>
-      </c>
-      <c r="E63">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>4</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>61</v>
       </c>
       <c r="B64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>304</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>308</v>
+      </c>
+      <c r="D64" t="s">
         <v>70</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>5</v>
       </c>
-      <c r="E64">
-        <f>IF(D64="float",4,IF(D64="byte",1,"Error"))*4</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <f>IF(E64="float",4,IF(E64="byte",1,"Error"))*4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>62</v>
       </c>
       <c r="B65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>308</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>312</v>
+      </c>
+      <c r="D65" t="s">
         <v>71</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>5</v>
       </c>
-      <c r="E65">
-        <f>IF(D65="float",4,IF(D65="byte",1,"Error"))*4</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <f>IF(E65="float",4,IF(E65="byte",1,"Error"))*4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>63</v>
       </c>
       <c r="B66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>312</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>313</v>
+      </c>
+      <c r="D66" t="s">
         <v>72</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>5</v>
       </c>
-      <c r="E66">
-        <f t="shared" si="0"/>
+      <c r="F66">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>64</v>
       </c>
       <c r="B67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>313</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67">
+        <f t="shared" si="0"/>
+        <v>314</v>
+      </c>
+      <c r="D67" t="s">
         <v>73</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>5</v>
       </c>
-      <c r="E67">
-        <f t="shared" si="0"/>
+      <c r="F67">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>65</v>
       </c>
       <c r="B68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>314</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68">
+        <f t="shared" ref="C68:C85" si="3">B68+F68</f>
+        <v>315</v>
+      </c>
+      <c r="D68" t="s">
         <v>74</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>5</v>
       </c>
-      <c r="E68">
-        <f t="shared" ref="E68:E85" si="2">IF(D68="float",4,IF(D68="byte",1,"Error"))</f>
+      <c r="F68">
+        <f t="shared" ref="F68:F84" si="4">IF(E68="float",4,IF(E68="byte",1,"Error"))</f>
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>66</v>
       </c>
       <c r="B69">
-        <f t="shared" ref="B69:B85" si="3">B68+E68</f>
+        <f t="shared" ref="B69:B85" si="5">B68+F68</f>
         <v>315</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69">
+        <f t="shared" si="3"/>
+        <v>316</v>
+      </c>
+      <c r="D69" t="s">
         <v>75</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>5</v>
       </c>
-      <c r="E69">
-        <f t="shared" si="2"/>
+      <c r="F69">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>67</v>
       </c>
       <c r="B70">
+        <f t="shared" si="5"/>
+        <v>316</v>
+      </c>
+      <c r="C70">
         <f t="shared" si="3"/>
-        <v>316</v>
-      </c>
-      <c r="C70" t="s">
+        <v>320</v>
+      </c>
+      <c r="D70" t="s">
         <v>76</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
         <v>5</v>
       </c>
-      <c r="E70">
-        <f>IF(D70="float",4,IF(D70="byte",1,"Error"))*4</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <f>IF(E70="float",4,IF(E70="byte",1,"Error"))*4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>68</v>
       </c>
       <c r="B71">
+        <f t="shared" si="5"/>
+        <v>320</v>
+      </c>
+      <c r="C71">
         <f t="shared" si="3"/>
-        <v>320</v>
-      </c>
-      <c r="C71" t="s">
+        <v>321</v>
+      </c>
+      <c r="D71" t="s">
         <v>77</v>
       </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
         <v>5</v>
       </c>
-      <c r="E71">
-        <f t="shared" si="2"/>
+      <c r="F71">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>69</v>
       </c>
       <c r="B72">
+        <f t="shared" si="5"/>
+        <v>321</v>
+      </c>
+      <c r="C72">
         <f t="shared" si="3"/>
-        <v>321</v>
-      </c>
-      <c r="C72" t="s">
+        <v>322</v>
+      </c>
+      <c r="D72" t="s">
         <v>78</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
         <v>5</v>
       </c>
-      <c r="E72">
-        <f t="shared" si="2"/>
+      <c r="F72">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>70</v>
       </c>
       <c r="B73">
+        <f t="shared" si="5"/>
+        <v>322</v>
+      </c>
+      <c r="C73">
         <f t="shared" si="3"/>
-        <v>322</v>
-      </c>
-      <c r="C73" t="s">
+        <v>323</v>
+      </c>
+      <c r="D73" t="s">
         <v>79</v>
       </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
         <v>5</v>
       </c>
-      <c r="E73">
-        <f t="shared" si="2"/>
+      <c r="F73">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>71</v>
       </c>
       <c r="B74">
+        <f t="shared" si="5"/>
+        <v>323</v>
+      </c>
+      <c r="C74">
         <f t="shared" si="3"/>
-        <v>323</v>
-      </c>
-      <c r="C74" t="s">
+        <v>324</v>
+      </c>
+      <c r="D74" t="s">
         <v>80</v>
       </c>
-      <c r="D74" t="s">
+      <c r="E74" t="s">
         <v>5</v>
       </c>
-      <c r="E74">
-        <f t="shared" si="2"/>
+      <c r="F74">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>72</v>
       </c>
       <c r="B75">
+        <f t="shared" si="5"/>
+        <v>324</v>
+      </c>
+      <c r="C75">
         <f t="shared" si="3"/>
-        <v>324</v>
-      </c>
-      <c r="C75" t="s">
+        <v>325</v>
+      </c>
+      <c r="D75" t="s">
         <v>81</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>5</v>
       </c>
-      <c r="E75">
-        <f t="shared" si="2"/>
+      <c r="F75">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>73</v>
       </c>
       <c r="B76">
+        <f t="shared" si="5"/>
+        <v>325</v>
+      </c>
+      <c r="C76">
         <f t="shared" si="3"/>
-        <v>325</v>
-      </c>
-      <c r="C76" t="s">
+        <v>326</v>
+      </c>
+      <c r="D76" t="s">
         <v>82</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>5</v>
       </c>
-      <c r="E76">
-        <f t="shared" si="2"/>
+      <c r="F76">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>74</v>
       </c>
       <c r="B77">
+        <f t="shared" si="5"/>
+        <v>326</v>
+      </c>
+      <c r="C77">
         <f t="shared" si="3"/>
-        <v>326</v>
-      </c>
-      <c r="C77" t="s">
+        <v>327</v>
+      </c>
+      <c r="D77" t="s">
         <v>83</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>5</v>
       </c>
-      <c r="E77">
-        <f t="shared" si="2"/>
+      <c r="F77">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>75</v>
       </c>
       <c r="B78">
+        <f t="shared" si="5"/>
+        <v>327</v>
+      </c>
+      <c r="C78">
         <f t="shared" si="3"/>
-        <v>327</v>
-      </c>
-      <c r="C78" t="s">
+        <v>328</v>
+      </c>
+      <c r="D78" t="s">
         <v>84</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>5</v>
       </c>
-      <c r="E78">
-        <f t="shared" si="2"/>
+      <c r="F78">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>76</v>
       </c>
       <c r="B79">
+        <f t="shared" si="5"/>
+        <v>328</v>
+      </c>
+      <c r="C79">
         <f t="shared" si="3"/>
-        <v>328</v>
-      </c>
-      <c r="C79" t="s">
+        <v>332</v>
+      </c>
+      <c r="D79" t="s">
         <v>85</v>
       </c>
-      <c r="D79" t="s">
-        <v>4</v>
-      </c>
-      <c r="E79">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E79" t="s">
+        <v>4</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>77</v>
       </c>
       <c r="B80">
+        <f t="shared" si="5"/>
+        <v>332</v>
+      </c>
+      <c r="C80">
         <f t="shared" si="3"/>
-        <v>332</v>
-      </c>
-      <c r="C80" t="s">
+        <v>333</v>
+      </c>
+      <c r="D80" t="s">
         <v>86</v>
       </c>
-      <c r="D80" t="s">
+      <c r="E80" t="s">
         <v>5</v>
       </c>
-      <c r="E80">
-        <f t="shared" si="2"/>
+      <c r="F80">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>78</v>
       </c>
       <c r="B81">
+        <f t="shared" si="5"/>
+        <v>333</v>
+      </c>
+      <c r="C81">
         <f t="shared" si="3"/>
-        <v>333</v>
-      </c>
-      <c r="C81" t="s">
+        <v>334</v>
+      </c>
+      <c r="D81" t="s">
         <v>87</v>
       </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>5</v>
       </c>
-      <c r="E81">
-        <f t="shared" si="2"/>
+      <c r="F81">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>79</v>
       </c>
       <c r="B82">
+        <f t="shared" si="5"/>
+        <v>334</v>
+      </c>
+      <c r="C82">
         <f t="shared" si="3"/>
-        <v>334</v>
-      </c>
-      <c r="C82" t="s">
+        <v>335</v>
+      </c>
+      <c r="D82" t="s">
         <v>88</v>
       </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
         <v>5</v>
       </c>
-      <c r="E82">
-        <f t="shared" si="2"/>
+      <c r="F82">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>80</v>
       </c>
       <c r="B83">
+        <f t="shared" si="5"/>
+        <v>335</v>
+      </c>
+      <c r="C83">
         <f t="shared" si="3"/>
-        <v>335</v>
-      </c>
-      <c r="C83" t="s">
+        <v>336</v>
+      </c>
+      <c r="D83" t="s">
         <v>89</v>
       </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>5</v>
       </c>
-      <c r="E83">
-        <f t="shared" si="2"/>
+      <c r="F83">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>81</v>
       </c>
       <c r="B84">
+        <f t="shared" si="5"/>
+        <v>336</v>
+      </c>
+      <c r="C84">
         <f t="shared" si="3"/>
-        <v>336</v>
-      </c>
-      <c r="C84" t="s">
+        <v>337</v>
+      </c>
+      <c r="D84" t="s">
         <v>90</v>
       </c>
-      <c r="D84" t="s">
+      <c r="E84" t="s">
         <v>5</v>
       </c>
-      <c r="E84">
-        <f t="shared" si="2"/>
+      <c r="F84">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>82</v>
       </c>
       <c r="B85">
+        <f t="shared" si="5"/>
+        <v>337</v>
+      </c>
+      <c r="C85">
         <f t="shared" si="3"/>
-        <v>337</v>
-      </c>
-      <c r="C85" t="s">
+        <v>1237</v>
+      </c>
+      <c r="D85" t="s">
         <v>107</v>
       </c>
-      <c r="E85">
-        <f>E106*20</f>
+      <c r="F85">
+        <f>F106*20</f>
         <v>900</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E86" s="2">
-        <f>SUM(E3:E85)</f>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F86" s="2">
+        <f>SUM(F3:F85)</f>
         <v>1237</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>91</v>
       </c>
@@ -2315,8 +2655,9 @@
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F89" s="1"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>83</v>
       </c>
@@ -2324,312 +2665,312 @@
         <f>B85</f>
         <v>337</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
         <v>92</v>
       </c>
-      <c r="D90" t="s">
-        <v>4</v>
-      </c>
-      <c r="E90">
-        <f>IF(D90="float",4,IF(D90="byte",1,"Error"))*3</f>
+      <c r="E90" t="s">
+        <v>4</v>
+      </c>
+      <c r="F90">
+        <f>IF(E90="float",4,IF(E90="byte",1,"Error"))*3</f>
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>84</v>
       </c>
       <c r="B91">
-        <f t="shared" ref="B91:B105" si="4">B90+E90</f>
+        <f t="shared" ref="B91:B105" si="6">B90+F90</f>
         <v>349</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
         <v>93</v>
       </c>
-      <c r="D91" t="s">
-        <v>4</v>
-      </c>
-      <c r="E91">
-        <f t="shared" ref="E90:E105" si="5">IF(D91="float",4,IF(D91="byte",1,"Error"))</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E91" t="s">
+        <v>4</v>
+      </c>
+      <c r="F91">
+        <f t="shared" ref="F91:F105" si="7">IF(E91="float",4,IF(E91="byte",1,"Error"))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>85</v>
       </c>
       <c r="B92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>353</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
         <v>94</v>
       </c>
-      <c r="D92" t="s">
-        <v>4</v>
-      </c>
-      <c r="E92">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E92" t="s">
+        <v>4</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>86</v>
       </c>
       <c r="B93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>357</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
         <v>95</v>
       </c>
-      <c r="D93" t="s">
-        <v>4</v>
-      </c>
-      <c r="E93">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E93" t="s">
+        <v>4</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>87</v>
       </c>
       <c r="B94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>361</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
         <v>96</v>
       </c>
-      <c r="D94" t="s">
-        <v>4</v>
-      </c>
-      <c r="E94">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E94" t="s">
+        <v>4</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>88</v>
       </c>
       <c r="B95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>365</v>
       </c>
-      <c r="C95" t="s">
+      <c r="D95" t="s">
         <v>97</v>
       </c>
-      <c r="D95" t="s">
-        <v>4</v>
-      </c>
-      <c r="E95">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E95" t="s">
+        <v>4</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>89</v>
       </c>
       <c r="B96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>369</v>
       </c>
-      <c r="C96" t="s">
+      <c r="D96" t="s">
         <v>0</v>
       </c>
-      <c r="D96" t="s">
-        <v>4</v>
-      </c>
-      <c r="E96">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E96" t="s">
+        <v>4</v>
+      </c>
+      <c r="F96">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>90</v>
       </c>
       <c r="B97">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>373</v>
       </c>
-      <c r="C97" t="s">
+      <c r="D97" t="s">
         <v>98</v>
       </c>
-      <c r="D97" t="s">
+      <c r="E97" t="s">
         <v>5</v>
       </c>
-      <c r="E97">
-        <f t="shared" si="5"/>
+      <c r="F97">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>91</v>
       </c>
       <c r="B98">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>374</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D98" t="s">
         <v>99</v>
       </c>
-      <c r="D98" t="s">
+      <c r="E98" t="s">
         <v>5</v>
       </c>
-      <c r="E98">
-        <f t="shared" si="5"/>
+      <c r="F98">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>92</v>
       </c>
       <c r="B99">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>375</v>
       </c>
-      <c r="C99" t="s">
+      <c r="D99" t="s">
         <v>100</v>
       </c>
-      <c r="D99" t="s">
+      <c r="E99" t="s">
         <v>5</v>
       </c>
-      <c r="E99">
-        <f t="shared" si="5"/>
+      <c r="F99">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>93</v>
       </c>
       <c r="B100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>376</v>
       </c>
-      <c r="C100" t="s">
+      <c r="D100" t="s">
         <v>101</v>
       </c>
-      <c r="D100" t="s">
+      <c r="E100" t="s">
         <v>5</v>
       </c>
-      <c r="E100">
-        <f t="shared" si="5"/>
+      <c r="F100">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>94</v>
       </c>
       <c r="B101">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>377</v>
       </c>
-      <c r="C101" t="s">
+      <c r="D101" t="s">
         <v>102</v>
       </c>
-      <c r="D101" t="s">
+      <c r="E101" t="s">
         <v>5</v>
       </c>
-      <c r="E101">
-        <f t="shared" si="5"/>
+      <c r="F101">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>95</v>
       </c>
       <c r="B102">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>378</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D102" t="s">
         <v>103</v>
       </c>
-      <c r="D102" t="s">
+      <c r="E102" t="s">
         <v>5</v>
       </c>
-      <c r="E102">
-        <f t="shared" si="5"/>
+      <c r="F102">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>96</v>
       </c>
       <c r="B103">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>379</v>
       </c>
-      <c r="C103" t="s">
+      <c r="D103" t="s">
         <v>104</v>
       </c>
-      <c r="D103" t="s">
+      <c r="E103" t="s">
         <v>5</v>
       </c>
-      <c r="E103">
-        <f t="shared" si="5"/>
+      <c r="F103">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>97</v>
       </c>
       <c r="B104">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>380</v>
       </c>
-      <c r="C104" t="s">
+      <c r="D104" t="s">
         <v>105</v>
       </c>
-      <c r="D104" t="s">
+      <c r="E104" t="s">
         <v>5</v>
       </c>
-      <c r="E104">
-        <f t="shared" si="5"/>
+      <c r="F104">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>98</v>
       </c>
       <c r="B105">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>381</v>
       </c>
-      <c r="C105" t="s">
+      <c r="D105" t="s">
         <v>106</v>
       </c>
-      <c r="D105" t="s">
+      <c r="E105" t="s">
         <v>5</v>
       </c>
-      <c r="E105">
-        <f t="shared" si="5"/>
+      <c r="F105">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E106" s="2">
-        <f>SUM(E90:E105)</f>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F106" s="2">
+        <f>SUM(F90:F105)</f>
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A89:E89"/>
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A89:F89"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished adding codemasters udp data
</commit_message>
<xml_diff>
--- a/artifacts/f12017/udp.xlsx
+++ b/artifacts/f12017/udp.xlsx
@@ -385,10 +385,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -692,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,13 +703,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -751,7 +751,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <f>B3+E3</f>
+        <f t="shared" ref="B4:B35" si="0">B3+E3</f>
         <v>4</v>
       </c>
       <c r="C4" t="s">
@@ -761,7 +761,7 @@
         <v>4</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E67" si="0">IF(D4="float",4,IF(D4="byte",1,"Error"))</f>
+        <f t="shared" ref="E4:E67" si="1">IF(D4="float",4,IF(D4="byte",1,"Error"))</f>
         <v>4</v>
       </c>
     </row>
@@ -770,7 +770,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <f>B4+E4</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C5" t="s">
@@ -780,7 +780,7 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -789,7 +789,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <f>B5+E5</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C6" t="s">
@@ -799,7 +799,7 @@
         <v>4</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -808,7 +808,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <f>B6+E6</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C7" t="s">
@@ -818,7 +818,7 @@
         <v>4</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -827,7 +827,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <f>B7+E7</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="C8" t="s">
@@ -837,7 +837,7 @@
         <v>4</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -846,7 +846,7 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <f>B8+E8</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="C9" t="s">
@@ -856,7 +856,7 @@
         <v>4</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -865,7 +865,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <f>B9+E9</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="C10" t="s">
@@ -875,7 +875,7 @@
         <v>4</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -884,7 +884,7 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <f>B10+E10</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="C11" t="s">
@@ -894,7 +894,7 @@
         <v>4</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -903,7 +903,7 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <f>B11+E11</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="C12" t="s">
@@ -913,7 +913,7 @@
         <v>4</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -922,7 +922,7 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <f>B12+E12</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="C13" t="s">
@@ -932,7 +932,7 @@
         <v>4</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -941,7 +941,7 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <f>B13+E13</f>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="C14" t="s">
@@ -951,7 +951,7 @@
         <v>4</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -960,7 +960,7 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <f>B14+E14</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="C15" t="s">
@@ -970,7 +970,7 @@
         <v>4</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -979,7 +979,7 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <f>B15+E15</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="C16" t="s">
@@ -989,7 +989,7 @@
         <v>4</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -998,7 +998,7 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <f>B16+E16</f>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="C17" t="s">
@@ -1008,7 +1008,7 @@
         <v>4</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <f>B17+E17</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="C18" t="s">
@@ -1027,7 +1027,7 @@
         <v>4</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1036,7 +1036,7 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <f>B18+E18</f>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="C19" t="s">
@@ -1046,7 +1046,7 @@
         <v>4</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1055,7 +1055,7 @@
         <v>17</v>
       </c>
       <c r="B20">
-        <f>B19+E19</f>
+        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="C20" t="s">
@@ -1074,7 +1074,7 @@
         <v>18</v>
       </c>
       <c r="B21">
-        <f>B20+E20</f>
+        <f t="shared" si="0"/>
         <v>84</v>
       </c>
       <c r="C21" t="s">
@@ -1093,7 +1093,7 @@
         <v>19</v>
       </c>
       <c r="B22">
-        <f>B21+E21</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="C22" t="s">
@@ -1112,7 +1112,7 @@
         <v>20</v>
       </c>
       <c r="B23">
-        <f>B22+E22</f>
+        <f t="shared" si="0"/>
         <v>116</v>
       </c>
       <c r="C23" t="s">
@@ -1122,7 +1122,7 @@
         <v>4</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1131,7 +1131,7 @@
         <v>21</v>
       </c>
       <c r="B24">
-        <f>B23+E23</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
       <c r="C24" t="s">
@@ -1141,7 +1141,7 @@
         <v>4</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1150,7 +1150,7 @@
         <v>22</v>
       </c>
       <c r="B25">
-        <f>B24+E24</f>
+        <f t="shared" si="0"/>
         <v>124</v>
       </c>
       <c r="C25" t="s">
@@ -1160,7 +1160,7 @@
         <v>4</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1169,7 +1169,7 @@
         <v>23</v>
       </c>
       <c r="B26">
-        <f>B25+E25</f>
+        <f t="shared" si="0"/>
         <v>128</v>
       </c>
       <c r="C26" t="s">
@@ -1179,7 +1179,7 @@
         <v>4</v>
       </c>
       <c r="E26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1188,7 +1188,7 @@
         <v>24</v>
       </c>
       <c r="B27">
-        <f>B26+E26</f>
+        <f t="shared" si="0"/>
         <v>132</v>
       </c>
       <c r="C27" t="s">
@@ -1198,7 +1198,7 @@
         <v>4</v>
       </c>
       <c r="E27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1207,7 +1207,7 @@
         <v>25</v>
       </c>
       <c r="B28">
-        <f>B27+E27</f>
+        <f t="shared" si="0"/>
         <v>136</v>
       </c>
       <c r="C28" t="s">
@@ -1217,7 +1217,7 @@
         <v>4</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1226,7 +1226,7 @@
         <v>26</v>
       </c>
       <c r="B29">
-        <f>B28+E28</f>
+        <f t="shared" si="0"/>
         <v>140</v>
       </c>
       <c r="C29" t="s">
@@ -1236,7 +1236,7 @@
         <v>4</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1245,7 +1245,7 @@
         <v>27</v>
       </c>
       <c r="B30">
-        <f>B29+E29</f>
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="C30" t="s">
@@ -1255,7 +1255,7 @@
         <v>4</v>
       </c>
       <c r="E30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1264,7 +1264,7 @@
         <v>28</v>
       </c>
       <c r="B31">
-        <f>B30+E30</f>
+        <f t="shared" si="0"/>
         <v>148</v>
       </c>
       <c r="C31" t="s">
@@ -1274,7 +1274,7 @@
         <v>4</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1283,7 +1283,7 @@
         <v>29</v>
       </c>
       <c r="B32">
-        <f>B31+E31</f>
+        <f t="shared" si="0"/>
         <v>152</v>
       </c>
       <c r="C32" t="s">
@@ -1293,7 +1293,7 @@
         <v>4</v>
       </c>
       <c r="E32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1302,7 +1302,7 @@
         <v>30</v>
       </c>
       <c r="B33">
-        <f>B32+E32</f>
+        <f t="shared" si="0"/>
         <v>156</v>
       </c>
       <c r="C33" t="s">
@@ -1312,7 +1312,7 @@
         <v>4</v>
       </c>
       <c r="E33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1321,7 +1321,7 @@
         <v>31</v>
       </c>
       <c r="B34">
-        <f>B33+E33</f>
+        <f t="shared" si="0"/>
         <v>160</v>
       </c>
       <c r="C34" t="s">
@@ -1331,7 +1331,7 @@
         <v>4</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1340,7 +1340,7 @@
         <v>32</v>
       </c>
       <c r="B35">
-        <f>B34+E34</f>
+        <f t="shared" si="0"/>
         <v>164</v>
       </c>
       <c r="C35" t="s">
@@ -1350,7 +1350,7 @@
         <v>4</v>
       </c>
       <c r="E35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1359,7 +1359,7 @@
         <v>33</v>
       </c>
       <c r="B36">
-        <f>B35+E35</f>
+        <f t="shared" ref="B36:B67" si="2">B35+E35</f>
         <v>168</v>
       </c>
       <c r="C36" t="s">
@@ -1369,7 +1369,7 @@
         <v>4</v>
       </c>
       <c r="E36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1378,7 +1378,7 @@
         <v>34</v>
       </c>
       <c r="B37">
-        <f>B36+E36</f>
+        <f t="shared" si="2"/>
         <v>172</v>
       </c>
       <c r="C37" t="s">
@@ -1388,7 +1388,7 @@
         <v>4</v>
       </c>
       <c r="E37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1397,7 +1397,7 @@
         <v>35</v>
       </c>
       <c r="B38">
-        <f>B37+E37</f>
+        <f t="shared" si="2"/>
         <v>176</v>
       </c>
       <c r="C38" t="s">
@@ -1407,7 +1407,7 @@
         <v>4</v>
       </c>
       <c r="E38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1416,7 +1416,7 @@
         <v>36</v>
       </c>
       <c r="B39">
-        <f>B38+E38</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="C39" t="s">
@@ -1426,7 +1426,7 @@
         <v>4</v>
       </c>
       <c r="E39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1435,7 +1435,7 @@
         <v>37</v>
       </c>
       <c r="B40">
-        <f>B39+E39</f>
+        <f t="shared" si="2"/>
         <v>184</v>
       </c>
       <c r="C40" t="s">
@@ -1445,7 +1445,7 @@
         <v>4</v>
       </c>
       <c r="E40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1454,7 +1454,7 @@
         <v>38</v>
       </c>
       <c r="B41">
-        <f>B40+E40</f>
+        <f t="shared" si="2"/>
         <v>188</v>
       </c>
       <c r="C41" t="s">
@@ -1464,7 +1464,7 @@
         <v>4</v>
       </c>
       <c r="E41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1473,7 +1473,7 @@
         <v>39</v>
       </c>
       <c r="B42">
-        <f>B41+E41</f>
+        <f t="shared" si="2"/>
         <v>192</v>
       </c>
       <c r="C42" t="s">
@@ -1483,7 +1483,7 @@
         <v>4</v>
       </c>
       <c r="E42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1492,7 +1492,7 @@
         <v>40</v>
       </c>
       <c r="B43">
-        <f>B42+E42</f>
+        <f t="shared" si="2"/>
         <v>196</v>
       </c>
       <c r="C43" t="s">
@@ -1502,7 +1502,7 @@
         <v>4</v>
       </c>
       <c r="E43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1511,7 +1511,7 @@
         <v>41</v>
       </c>
       <c r="B44">
-        <f>B43+E43</f>
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
       <c r="C44" t="s">
@@ -1521,7 +1521,7 @@
         <v>4</v>
       </c>
       <c r="E44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1530,7 +1530,7 @@
         <v>42</v>
       </c>
       <c r="B45">
-        <f>B44+E44</f>
+        <f t="shared" si="2"/>
         <v>204</v>
       </c>
       <c r="C45" t="s">
@@ -1549,7 +1549,7 @@
         <v>43</v>
       </c>
       <c r="B46">
-        <f>B45+E45</f>
+        <f t="shared" si="2"/>
         <v>220</v>
       </c>
       <c r="C46" t="s">
@@ -1568,7 +1568,7 @@
         <v>44</v>
       </c>
       <c r="B47">
-        <f>B46+E46</f>
+        <f t="shared" si="2"/>
         <v>236</v>
       </c>
       <c r="C47" t="s">
@@ -1578,7 +1578,7 @@
         <v>4</v>
       </c>
       <c r="E47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1587,7 +1587,7 @@
         <v>45</v>
       </c>
       <c r="B48">
-        <f>B47+E47</f>
+        <f t="shared" si="2"/>
         <v>240</v>
       </c>
       <c r="C48" t="s">
@@ -1597,7 +1597,7 @@
         <v>4</v>
       </c>
       <c r="E48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1606,7 +1606,7 @@
         <v>46</v>
       </c>
       <c r="B49">
-        <f>B48+E48</f>
+        <f t="shared" si="2"/>
         <v>244</v>
       </c>
       <c r="C49" t="s">
@@ -1616,7 +1616,7 @@
         <v>4</v>
       </c>
       <c r="E49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1625,7 +1625,7 @@
         <v>47</v>
       </c>
       <c r="B50">
-        <f>B49+E49</f>
+        <f t="shared" si="2"/>
         <v>248</v>
       </c>
       <c r="C50" t="s">
@@ -1635,7 +1635,7 @@
         <v>4</v>
       </c>
       <c r="E50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1644,7 +1644,7 @@
         <v>48</v>
       </c>
       <c r="B51">
-        <f>B50+E50</f>
+        <f t="shared" si="2"/>
         <v>252</v>
       </c>
       <c r="C51" t="s">
@@ -1654,7 +1654,7 @@
         <v>4</v>
       </c>
       <c r="E51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1663,7 +1663,7 @@
         <v>49</v>
       </c>
       <c r="B52">
-        <f>B51+E51</f>
+        <f t="shared" si="2"/>
         <v>256</v>
       </c>
       <c r="C52" t="s">
@@ -1673,7 +1673,7 @@
         <v>4</v>
       </c>
       <c r="E52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1682,7 +1682,7 @@
         <v>50</v>
       </c>
       <c r="B53">
-        <f>B52+E52</f>
+        <f t="shared" si="2"/>
         <v>260</v>
       </c>
       <c r="C53" t="s">
@@ -1692,7 +1692,7 @@
         <v>4</v>
       </c>
       <c r="E53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1701,7 +1701,7 @@
         <v>51</v>
       </c>
       <c r="B54">
-        <f>B53+E53</f>
+        <f t="shared" si="2"/>
         <v>264</v>
       </c>
       <c r="C54" t="s">
@@ -1711,7 +1711,7 @@
         <v>4</v>
       </c>
       <c r="E54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1720,7 +1720,7 @@
         <v>52</v>
       </c>
       <c r="B55">
-        <f>B54+E54</f>
+        <f t="shared" si="2"/>
         <v>268</v>
       </c>
       <c r="C55" t="s">
@@ -1730,7 +1730,7 @@
         <v>4</v>
       </c>
       <c r="E55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1739,7 +1739,7 @@
         <v>53</v>
       </c>
       <c r="B56">
-        <f>B55+E55</f>
+        <f t="shared" si="2"/>
         <v>272</v>
       </c>
       <c r="C56" t="s">
@@ -1749,7 +1749,7 @@
         <v>4</v>
       </c>
       <c r="E56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1758,7 +1758,7 @@
         <v>54</v>
       </c>
       <c r="B57">
-        <f>B56+E56</f>
+        <f t="shared" si="2"/>
         <v>276</v>
       </c>
       <c r="C57" t="s">
@@ -1768,7 +1768,7 @@
         <v>4</v>
       </c>
       <c r="E57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1777,7 +1777,7 @@
         <v>55</v>
       </c>
       <c r="B58">
-        <f>B57+E57</f>
+        <f t="shared" si="2"/>
         <v>280</v>
       </c>
       <c r="C58" t="s">
@@ -1787,7 +1787,7 @@
         <v>4</v>
       </c>
       <c r="E58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1796,7 +1796,7 @@
         <v>56</v>
       </c>
       <c r="B59">
-        <f>B58+E58</f>
+        <f t="shared" si="2"/>
         <v>284</v>
       </c>
       <c r="C59" t="s">
@@ -1806,7 +1806,7 @@
         <v>4</v>
       </c>
       <c r="E59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1815,7 +1815,7 @@
         <v>57</v>
       </c>
       <c r="B60">
-        <f>B59+E59</f>
+        <f t="shared" si="2"/>
         <v>288</v>
       </c>
       <c r="C60" t="s">
@@ -1825,7 +1825,7 @@
         <v>4</v>
       </c>
       <c r="E60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1834,7 +1834,7 @@
         <v>58</v>
       </c>
       <c r="B61">
-        <f>B60+E60</f>
+        <f t="shared" si="2"/>
         <v>292</v>
       </c>
       <c r="C61" t="s">
@@ -1844,7 +1844,7 @@
         <v>4</v>
       </c>
       <c r="E61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1853,7 +1853,7 @@
         <v>59</v>
       </c>
       <c r="B62">
-        <f>B61+E61</f>
+        <f t="shared" si="2"/>
         <v>296</v>
       </c>
       <c r="C62" t="s">
@@ -1863,7 +1863,7 @@
         <v>4</v>
       </c>
       <c r="E62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1872,7 +1872,7 @@
         <v>60</v>
       </c>
       <c r="B63">
-        <f>B62+E62</f>
+        <f t="shared" si="2"/>
         <v>300</v>
       </c>
       <c r="C63" t="s">
@@ -1882,7 +1882,7 @@
         <v>4</v>
       </c>
       <c r="E63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -1891,7 +1891,7 @@
         <v>61</v>
       </c>
       <c r="B64">
-        <f>B63+E63</f>
+        <f t="shared" si="2"/>
         <v>304</v>
       </c>
       <c r="C64" t="s">
@@ -1910,7 +1910,7 @@
         <v>62</v>
       </c>
       <c r="B65">
-        <f>B64+E64</f>
+        <f t="shared" si="2"/>
         <v>308</v>
       </c>
       <c r="C65" t="s">
@@ -1929,7 +1929,7 @@
         <v>63</v>
       </c>
       <c r="B66">
-        <f>B65+E65</f>
+        <f t="shared" si="2"/>
         <v>312</v>
       </c>
       <c r="C66" t="s">
@@ -1939,7 +1939,7 @@
         <v>5</v>
       </c>
       <c r="E66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1948,7 +1948,7 @@
         <v>64</v>
       </c>
       <c r="B67">
-        <f>B66+E66</f>
+        <f t="shared" si="2"/>
         <v>313</v>
       </c>
       <c r="C67" t="s">
@@ -1958,7 +1958,7 @@
         <v>5</v>
       </c>
       <c r="E67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1967,7 +1967,7 @@
         <v>65</v>
       </c>
       <c r="B68">
-        <f>B67+E67</f>
+        <f t="shared" ref="B68:B85" si="3">B67+E67</f>
         <v>314</v>
       </c>
       <c r="C68" t="s">
@@ -1977,7 +1977,7 @@
         <v>5</v>
       </c>
       <c r="E68">
-        <f t="shared" ref="E68:E84" si="1">IF(D68="float",4,IF(D68="byte",1,"Error"))</f>
+        <f t="shared" ref="E68:E84" si="4">IF(D68="float",4,IF(D68="byte",1,"Error"))</f>
         <v>1</v>
       </c>
     </row>
@@ -1986,7 +1986,7 @@
         <v>66</v>
       </c>
       <c r="B69">
-        <f>B68+E68</f>
+        <f t="shared" si="3"/>
         <v>315</v>
       </c>
       <c r="C69" t="s">
@@ -1996,7 +1996,7 @@
         <v>5</v>
       </c>
       <c r="E69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -2005,7 +2005,7 @@
         <v>67</v>
       </c>
       <c r="B70">
-        <f>B69+E69</f>
+        <f t="shared" si="3"/>
         <v>316</v>
       </c>
       <c r="C70" t="s">
@@ -2024,7 +2024,7 @@
         <v>68</v>
       </c>
       <c r="B71">
-        <f>B70+E70</f>
+        <f t="shared" si="3"/>
         <v>320</v>
       </c>
       <c r="C71" t="s">
@@ -2034,7 +2034,7 @@
         <v>5</v>
       </c>
       <c r="E71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -2043,7 +2043,7 @@
         <v>69</v>
       </c>
       <c r="B72">
-        <f>B71+E71</f>
+        <f t="shared" si="3"/>
         <v>321</v>
       </c>
       <c r="C72" t="s">
@@ -2053,7 +2053,7 @@
         <v>5</v>
       </c>
       <c r="E72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -2062,7 +2062,7 @@
         <v>70</v>
       </c>
       <c r="B73">
-        <f>B72+E72</f>
+        <f t="shared" si="3"/>
         <v>322</v>
       </c>
       <c r="C73" t="s">
@@ -2072,7 +2072,7 @@
         <v>5</v>
       </c>
       <c r="E73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -2081,7 +2081,7 @@
         <v>71</v>
       </c>
       <c r="B74">
-        <f>B73+E73</f>
+        <f t="shared" si="3"/>
         <v>323</v>
       </c>
       <c r="C74" t="s">
@@ -2091,7 +2091,7 @@
         <v>5</v>
       </c>
       <c r="E74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -2100,7 +2100,7 @@
         <v>72</v>
       </c>
       <c r="B75">
-        <f>B74+E74</f>
+        <f t="shared" si="3"/>
         <v>324</v>
       </c>
       <c r="C75" t="s">
@@ -2110,7 +2110,7 @@
         <v>5</v>
       </c>
       <c r="E75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -2119,7 +2119,7 @@
         <v>73</v>
       </c>
       <c r="B76">
-        <f>B75+E75</f>
+        <f t="shared" si="3"/>
         <v>325</v>
       </c>
       <c r="C76" t="s">
@@ -2129,7 +2129,7 @@
         <v>5</v>
       </c>
       <c r="E76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -2138,7 +2138,7 @@
         <v>74</v>
       </c>
       <c r="B77">
-        <f>B76+E76</f>
+        <f t="shared" si="3"/>
         <v>326</v>
       </c>
       <c r="C77" t="s">
@@ -2148,7 +2148,7 @@
         <v>5</v>
       </c>
       <c r="E77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -2157,7 +2157,7 @@
         <v>75</v>
       </c>
       <c r="B78">
-        <f>B77+E77</f>
+        <f t="shared" si="3"/>
         <v>327</v>
       </c>
       <c r="C78" t="s">
@@ -2167,7 +2167,7 @@
         <v>5</v>
       </c>
       <c r="E78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -2176,7 +2176,7 @@
         <v>76</v>
       </c>
       <c r="B79">
-        <f>B78+E78</f>
+        <f t="shared" si="3"/>
         <v>328</v>
       </c>
       <c r="C79" t="s">
@@ -2186,7 +2186,7 @@
         <v>4</v>
       </c>
       <c r="E79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
     </row>
@@ -2195,7 +2195,7 @@
         <v>77</v>
       </c>
       <c r="B80">
-        <f>B79+E79</f>
+        <f t="shared" si="3"/>
         <v>332</v>
       </c>
       <c r="C80" t="s">
@@ -2205,7 +2205,7 @@
         <v>5</v>
       </c>
       <c r="E80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -2214,7 +2214,7 @@
         <v>78</v>
       </c>
       <c r="B81">
-        <f>B80+E80</f>
+        <f t="shared" si="3"/>
         <v>333</v>
       </c>
       <c r="C81" t="s">
@@ -2224,7 +2224,7 @@
         <v>5</v>
       </c>
       <c r="E81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -2233,7 +2233,7 @@
         <v>79</v>
       </c>
       <c r="B82">
-        <f>B81+E81</f>
+        <f t="shared" si="3"/>
         <v>334</v>
       </c>
       <c r="C82" t="s">
@@ -2243,7 +2243,7 @@
         <v>5</v>
       </c>
       <c r="E82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -2252,7 +2252,7 @@
         <v>80</v>
       </c>
       <c r="B83">
-        <f>B82+E82</f>
+        <f t="shared" si="3"/>
         <v>335</v>
       </c>
       <c r="C83" t="s">
@@ -2262,7 +2262,7 @@
         <v>5</v>
       </c>
       <c r="E83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -2271,7 +2271,7 @@
         <v>81</v>
       </c>
       <c r="B84">
-        <f>B83+E83</f>
+        <f t="shared" si="3"/>
         <v>336</v>
       </c>
       <c r="C84" t="s">
@@ -2281,7 +2281,7 @@
         <v>5</v>
       </c>
       <c r="E84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -2290,7 +2290,7 @@
         <v>82</v>
       </c>
       <c r="B85">
-        <f>B84+E84</f>
+        <f t="shared" si="3"/>
         <v>337</v>
       </c>
       <c r="C85" t="s">
@@ -2302,27 +2302,26 @@
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E86" s="2">
+      <c r="E86" s="1">
         <f>SUM(E3:E85)</f>
         <v>1237</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+      <c r="A89" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B89" s="1"/>
-      <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
-      <c r="E89" s="1"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>83</v>
       </c>
       <c r="B90">
-        <f>B85</f>
-        <v>337</v>
+        <v>0</v>
       </c>
       <c r="C90" t="s">
         <v>92</v>
@@ -2340,8 +2339,8 @@
         <v>84</v>
       </c>
       <c r="B91">
-        <f>B90+E90</f>
-        <v>349</v>
+        <f t="shared" ref="B91:B105" si="5">B90+E90</f>
+        <v>12</v>
       </c>
       <c r="C91" t="s">
         <v>93</v>
@@ -2350,7 +2349,7 @@
         <v>4</v>
       </c>
       <c r="E91">
-        <f t="shared" ref="E91:E105" si="2">IF(D91="float",4,IF(D91="byte",1,"Error"))</f>
+        <f t="shared" ref="E91:E105" si="6">IF(D91="float",4,IF(D91="byte",1,"Error"))</f>
         <v>4</v>
       </c>
     </row>
@@ -2359,8 +2358,8 @@
         <v>85</v>
       </c>
       <c r="B92">
-        <f>B91+E91</f>
-        <v>353</v>
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
       <c r="C92" t="s">
         <v>94</v>
@@ -2369,7 +2368,7 @@
         <v>4</v>
       </c>
       <c r="E92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
     </row>
@@ -2378,8 +2377,8 @@
         <v>86</v>
       </c>
       <c r="B93">
-        <f>B92+E92</f>
-        <v>357</v>
+        <f t="shared" si="5"/>
+        <v>20</v>
       </c>
       <c r="C93" t="s">
         <v>95</v>
@@ -2388,7 +2387,7 @@
         <v>4</v>
       </c>
       <c r="E93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
     </row>
@@ -2397,8 +2396,8 @@
         <v>87</v>
       </c>
       <c r="B94">
-        <f>B93+E93</f>
-        <v>361</v>
+        <f t="shared" si="5"/>
+        <v>24</v>
       </c>
       <c r="C94" t="s">
         <v>96</v>
@@ -2407,7 +2406,7 @@
         <v>4</v>
       </c>
       <c r="E94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
     </row>
@@ -2416,8 +2415,8 @@
         <v>88</v>
       </c>
       <c r="B95">
-        <f>B94+E94</f>
-        <v>365</v>
+        <f t="shared" si="5"/>
+        <v>28</v>
       </c>
       <c r="C95" t="s">
         <v>97</v>
@@ -2426,7 +2425,7 @@
         <v>4</v>
       </c>
       <c r="E95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
     </row>
@@ -2435,8 +2434,8 @@
         <v>89</v>
       </c>
       <c r="B96">
-        <f>B95+E95</f>
-        <v>369</v>
+        <f t="shared" si="5"/>
+        <v>32</v>
       </c>
       <c r="C96" t="s">
         <v>0</v>
@@ -2445,7 +2444,7 @@
         <v>4</v>
       </c>
       <c r="E96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
     </row>
@@ -2454,8 +2453,8 @@
         <v>90</v>
       </c>
       <c r="B97">
-        <f>B96+E96</f>
-        <v>373</v>
+        <f t="shared" si="5"/>
+        <v>36</v>
       </c>
       <c r="C97" t="s">
         <v>98</v>
@@ -2464,7 +2463,7 @@
         <v>5</v>
       </c>
       <c r="E97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -2473,8 +2472,8 @@
         <v>91</v>
       </c>
       <c r="B98">
-        <f>B97+E97</f>
-        <v>374</v>
+        <f t="shared" si="5"/>
+        <v>37</v>
       </c>
       <c r="C98" t="s">
         <v>99</v>
@@ -2483,7 +2482,7 @@
         <v>5</v>
       </c>
       <c r="E98">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -2492,8 +2491,8 @@
         <v>92</v>
       </c>
       <c r="B99">
-        <f>B98+E98</f>
-        <v>375</v>
+        <f t="shared" si="5"/>
+        <v>38</v>
       </c>
       <c r="C99" t="s">
         <v>100</v>
@@ -2502,7 +2501,7 @@
         <v>5</v>
       </c>
       <c r="E99">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -2511,8 +2510,8 @@
         <v>93</v>
       </c>
       <c r="B100">
-        <f>B99+E99</f>
-        <v>376</v>
+        <f t="shared" si="5"/>
+        <v>39</v>
       </c>
       <c r="C100" t="s">
         <v>101</v>
@@ -2521,7 +2520,7 @@
         <v>5</v>
       </c>
       <c r="E100">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -2530,8 +2529,8 @@
         <v>94</v>
       </c>
       <c r="B101">
-        <f>B100+E100</f>
-        <v>377</v>
+        <f t="shared" si="5"/>
+        <v>40</v>
       </c>
       <c r="C101" t="s">
         <v>102</v>
@@ -2540,7 +2539,7 @@
         <v>5</v>
       </c>
       <c r="E101">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -2549,8 +2548,8 @@
         <v>95</v>
       </c>
       <c r="B102">
-        <f>B101+E101</f>
-        <v>378</v>
+        <f t="shared" si="5"/>
+        <v>41</v>
       </c>
       <c r="C102" t="s">
         <v>103</v>
@@ -2559,7 +2558,7 @@
         <v>5</v>
       </c>
       <c r="E102">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -2568,8 +2567,8 @@
         <v>96</v>
       </c>
       <c r="B103">
-        <f>B102+E102</f>
-        <v>379</v>
+        <f t="shared" si="5"/>
+        <v>42</v>
       </c>
       <c r="C103" t="s">
         <v>104</v>
@@ -2578,7 +2577,7 @@
         <v>5</v>
       </c>
       <c r="E103">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -2587,8 +2586,8 @@
         <v>97</v>
       </c>
       <c r="B104">
-        <f>B103+E103</f>
-        <v>380</v>
+        <f t="shared" si="5"/>
+        <v>43</v>
       </c>
       <c r="C104" t="s">
         <v>105</v>
@@ -2597,7 +2596,7 @@
         <v>5</v>
       </c>
       <c r="E104">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -2606,8 +2605,8 @@
         <v>98</v>
       </c>
       <c r="B105">
-        <f>B104+E104</f>
-        <v>381</v>
+        <f t="shared" si="5"/>
+        <v>44</v>
       </c>
       <c r="C105" t="s">
         <v>106</v>
@@ -2616,12 +2615,12 @@
         <v>5</v>
       </c>
       <c r="E105">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E106" s="2">
+      <c r="E106" s="1">
         <f>SUM(E90:E105)</f>
         <v>45</v>
       </c>

</xml_diff>